<commit_message>
- webapp追加 - ErrorProp, writable追加 - 不要module削除 - build Debug82, Release82追加
</commit_message>
<xml_diff>
--- a/paramTable.xlsx
+++ b/paramTable.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3092" uniqueCount="1699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3090" uniqueCount="1699">
   <si>
     <r>
       <t>0</t>
@@ -6619,9 +6619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -10988,7 +10988,7 @@
         <v>101</v>
       </c>
       <c r="E113" s="18" t="str">
-        <f t="shared" ref="E113:E144" si="6">LOWER(MID(F113,1,1))&amp;MID(F113,2,999)</f>
+        <f t="shared" ref="E113:E127" si="6">LOWER(MID(F113,1,1))&amp;MID(F113,2,999)</f>
         <v>dispMode</v>
       </c>
       <c r="F113" s="10" t="str">
@@ -11415,9 +11415,7 @@
         <v>ExposureBiasCompensation</v>
       </c>
       <c r="G123" s="1"/>
-      <c r="H123" s="12" t="s">
-        <v>121</v>
-      </c>
+      <c r="H123" s="12"/>
       <c r="I123" s="4" t="s">
         <v>12</v>
       </c>
@@ -11753,9 +11751,7 @@
         <v>FlashCompensation</v>
       </c>
       <c r="G130" s="1"/>
-      <c r="H130" s="12" t="s">
-        <v>147</v>
-      </c>
+      <c r="H130" s="12"/>
       <c r="I130" s="4" t="s">
         <v>12</v>
       </c>
@@ -19486,7 +19482,7 @@
     </row>
     <row r="329" spans="1:20" x14ac:dyDescent="0.2">
       <c r="E329" s="18" t="str">
-        <f t="shared" ref="E329:E360" si="18">LOWER(MID(F329,1,1))&amp;MID(F329,2,999)</f>
+        <f t="shared" ref="E329:E334" si="18">LOWER(MID(F329,1,1))&amp;MID(F329,2,999)</f>
         <v>recordingState</v>
       </c>
       <c r="F329" s="10" t="str">
@@ -22216,7 +22212,7 @@
         <v>440</v>
       </c>
       <c r="E400" s="18" t="str">
-        <f t="shared" ref="E400:E431" si="22">LOWER(MID(F400,1,1))&amp;MID(F400,2,999)</f>
+        <f t="shared" ref="E400:E401" si="22">LOWER(MID(F400,1,1))&amp;MID(F400,2,999)</f>
         <v>zoomDistance</v>
       </c>
       <c r="F400" s="19" t="str">

</xml_diff>